<commit_message>
change format excel import user
</commit_message>
<xml_diff>
--- a/assets/media/sertif.xlsx
+++ b/assets/media/sertif.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">uname</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">fullname</t>
   </si>
   <si>
-    <t xml:space="preserve">is_active</t>
+    <t xml:space="preserve">telepon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pekerjaan</t>
   </si>
   <si>
     <t xml:space="preserve">bod</t>
@@ -41,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">XNXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">administrator</t>
@@ -170,21 +170,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -208,105 +200,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -315,12 +299,9 @@
       <c r="C7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -328,9 +309,6 @@
       </c>
       <c r="C8" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>